<commit_message>
height does not change on band resize and new colors
</commit_message>
<xml_diff>
--- a/v1/data/formatted-data.xlsx
+++ b/v1/data/formatted-data.xlsx
@@ -5,20 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellecarrick/Desktop/PROJECTS/data-leaks/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellecarrick/Desktop/PROJECTS/data-leaks/v1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="19960" windowHeight="17060" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="19960" windowHeight="17060" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="graphs" sheetId="7" r:id="rId1"/>
     <sheet name="timeseries_reformat" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="9" r:id="rId3"/>
     <sheet name="data.json" sheetId="8" r:id="rId4"/>
-    <sheet name="Raw" sheetId="1" r:id="rId5"/>
-    <sheet name="Raw 2017" sheetId="5" r:id="rId6"/>
-    <sheet name="Data_sources" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId5"/>
+    <sheet name="Raw" sheetId="1" r:id="rId6"/>
+    <sheet name="Raw 2017" sheetId="5" r:id="rId7"/>
+    <sheet name="Data_sources" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2244" uniqueCount="296">
   <si>
     <t>Entity</t>
   </si>
@@ -1598,9 +1599,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="71">
@@ -1812,8 +1814,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2259,7 +2262,7 @@
   </sheetPr>
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:C58"/>
     </sheetView>
   </sheetViews>
@@ -3737,8 +3740,8 @@
   </sheetPr>
   <dimension ref="A1:J807"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A544" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I561"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection sqref="A1:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14707,6 +14710,640 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="1"/>
+  </sheetPr>
+  <dimension ref="A1:C56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>2007</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2007</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2007</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2007</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>2007</v>
+      </c>
+      <c r="B6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>2008</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>2008</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>2008</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>2008</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>2008</v>
+      </c>
+      <c r="B11" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>2009</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>2009</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>2009</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>2009</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>2009</v>
+      </c>
+      <c r="B16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C16">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>2010</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>2010</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>2010</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>2010</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>2010</v>
+      </c>
+      <c r="B21" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>2011</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>2011</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24">
+        <v>2011</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25">
+        <v>2011</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26">
+        <v>2011</v>
+      </c>
+      <c r="B26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27">
+        <v>2012</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28">
+        <v>2012</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29">
+        <v>2012</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>2012</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>2012</v>
+      </c>
+      <c r="B31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>2013</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33">
+        <v>2013</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34">
+        <v>2013</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35">
+        <v>2013</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36">
+        <v>2013</v>
+      </c>
+      <c r="B36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C36">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37">
+        <v>2014</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38">
+        <v>2014</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>2014</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>2014</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41">
+        <v>2014</v>
+      </c>
+      <c r="B41" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42">
+        <v>2015</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43">
+        <v>2015</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44">
+        <v>2015</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45">
+        <v>2015</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46">
+        <v>2015</v>
+      </c>
+      <c r="B46" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47">
+        <v>2016</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48">
+        <v>2016</v>
+      </c>
+      <c r="B48" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49">
+        <v>2016</v>
+      </c>
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50">
+        <v>2016</v>
+      </c>
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51">
+        <v>2016</v>
+      </c>
+      <c r="B51" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A52">
+        <v>2017</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A53">
+        <v>2017</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A54">
+        <v>2017</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A55">
+        <v>2017</v>
+      </c>
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A56">
+        <v>2017</v>
+      </c>
+      <c r="B56" t="s">
+        <v>140</v>
+      </c>
+      <c r="C56">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="1"/>
@@ -17142,7 +17779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="1"/>
@@ -17617,7 +18254,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="3" tint="0.39997558519241921"/>

</xml_diff>

<commit_message>
we have 5 chartrs rendering, yayyyyy
</commit_message>
<xml_diff>
--- a/v1/data/formatted-data.xlsx
+++ b/v1/data/formatted-data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28109"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniellecarrick/Desktop/PROJECTS/data-leaks/v1/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcarrick/Desktop/WIRED/data-leaks/v1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="19960" windowHeight="17060" activeTab="4"/>
+    <workbookView xWindow="280" yWindow="740" windowWidth="25640" windowHeight="16220" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="graphs" sheetId="7" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="Raw 2017" sheetId="5" r:id="rId7"/>
     <sheet name="Data_sources" sheetId="6" r:id="rId8"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet1!$B$1:$B$56</definedName>
+  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -14717,7 +14720,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C46" sqref="C46:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -14738,142 +14741,142 @@
         <v>2007</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>27</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>63</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4">
-        <v>2007</v>
+        <v>2009</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>123</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5">
-        <v>2007</v>
+        <v>2010</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5">
-        <v>90</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6">
-        <v>2007</v>
+        <v>2011</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>102</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8">
-        <v>2008</v>
+        <v>2013</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>91</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9">
-        <v>2008</v>
+        <v>2014</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>137</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>2008</v>
+        <v>2015</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
-        <v>95</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>2008</v>
+        <v>2016</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>2009</v>
+        <v>2017</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>85</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C13">
-        <v>97</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14">
-        <v>78</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
@@ -14881,153 +14884,153 @@
         <v>2009</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>37</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C17">
-        <v>102</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18">
-        <v>113</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19">
-        <v>111</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23">
-        <v>2011</v>
+        <v>2017</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>110</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C25">
-        <v>45</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>8</v>
       </c>
       <c r="C26">
-        <v>32</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27">
-        <v>40</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
       <c r="C28">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
@@ -15035,153 +15038,153 @@
         <v>2012</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C29">
-        <v>57</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C30">
-        <v>41</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="B31" t="s">
-        <v>140</v>
+        <v>8</v>
       </c>
       <c r="C31">
-        <v>54</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C32">
-        <v>72</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
       <c r="C33">
-        <v>160</v>
+        <v>607</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34">
-        <v>2013</v>
+        <v>2017</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C34">
-        <v>79</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C35">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36">
-        <v>2013</v>
+        <v>2008</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>7</v>
       </c>
       <c r="C36">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
       </c>
       <c r="C37">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38">
-        <v>231</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C39">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C40">
-        <v>92</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B41" t="s">
-        <v>140</v>
+        <v>7</v>
       </c>
       <c r="C41">
-        <v>117</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
@@ -15189,142 +15192,142 @@
         <v>2015</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <v>295</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <v>109</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46">
-        <v>2015</v>
+        <v>2007</v>
       </c>
       <c r="B46" t="s">
         <v>140</v>
       </c>
       <c r="C46">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>140</v>
       </c>
       <c r="C47">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48">
-        <v>2016</v>
+        <v>2009</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>140</v>
       </c>
       <c r="C48">
-        <v>607</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>140</v>
       </c>
       <c r="C49">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
       <c r="C50">
-        <v>101</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="B51" t="s">
         <v>140</v>
       </c>
       <c r="C51">
-        <v>70</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52">
-        <v>2017</v>
+        <v>2013</v>
       </c>
       <c r="B52" t="s">
-        <v>7</v>
+        <v>140</v>
       </c>
       <c r="C52">
-        <v>64</v>
+        <v>89</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>140</v>
       </c>
       <c r="C53">
-        <v>1002</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>140</v>
       </c>
       <c r="C54">
-        <v>42</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>140</v>
       </c>
       <c r="C55">
-        <v>106</v>
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
@@ -15339,6 +15342,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B56">
+    <sortState ref="A2:C56">
+      <sortCondition ref="B1:B56"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>